<commit_message>
Comlete testing run to get valid test times.
</commit_message>
<xml_diff>
--- a/dev-topics-codingexams/dev-topics-amazon-rangeconsolidator/analytics/raw_data/test_run.xlsx
+++ b/dev-topics-codingexams/dev-topics-amazon-rangeconsolidator/analytics/raw_data/test_run.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="13">
   <si>
     <t>case</t>
   </si>
@@ -44,28 +44,24 @@
     <t>u_nano</t>
   </si>
   <si>
-    <t>Ratio</t>
-  </si>
-  <si>
     <t>nLogn/10K</t>
   </si>
   <si>
-    <t xml:space="preserve"> L2Rx10</t>
+    <t>nLogn/100K</t>
   </si>
   <si>
-    <t xml:space="preserve"> R2Lx10</t>
+    <t xml:space="preserve"> L2R10x</t>
   </si>
   <si>
-    <t>nLogn/100K</t>
+    <t xml:space="preserve"> R2L10x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -545,14 +541,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -646,7 +640,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -714,45 +708,45 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>444</c:v>
+                  <c:v>522.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>471.7</c:v>
+                  <c:v>417</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>295.3</c:v>
+                  <c:v>476.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>332.5</c:v>
+                  <c:v>291.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>318.39999999999998</c:v>
+                  <c:v>354.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>345.5</c:v>
+                  <c:v>370.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>377.7</c:v>
+                  <c:v>418</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>406.7</c:v>
+                  <c:v>477.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>470.1</c:v>
+                  <c:v>493</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>489.2</c:v>
+                  <c:v>511.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>541.29999999999995</c:v>
+                  <c:v>565.79999999999995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>596.4</c:v>
+                  <c:v>622.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -820,45 +814,45 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>190.9</c:v>
+                  <c:v>197.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>167.7</c:v>
+                  <c:v>224.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>149.19999999999999</c:v>
+                  <c:v>151.80000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>149.1</c:v>
+                  <c:v>158.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150.9</c:v>
+                  <c:v>162.80000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>150.30000000000001</c:v>
+                  <c:v>155.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.80000000000001</c:v>
+                  <c:v>155.80000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>155.69999999999999</c:v>
+                  <c:v>174.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>153.4</c:v>
+                  <c:v>159.30000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>151.69999999999999</c:v>
+                  <c:v>166.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>153.80000000000001</c:v>
+                  <c:v>167.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>163.1</c:v>
+                  <c:v>166.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -868,18 +862,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125691392"/>
-        <c:axId val="125693312"/>
+        <c:axId val="126870272"/>
+        <c:axId val="126872192"/>
       </c:scatterChart>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>test_run!$H$1</c:f>
+              <c:f>test_run!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -935,7 +929,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>test_run!$H$2:$H$13</c:f>
+              <c:f>test_run!$G$2:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -978,7 +972,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -988,11 +982,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="126295424"/>
-        <c:axId val="126293504"/>
+        <c:axId val="149549440"/>
+        <c:axId val="149753856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125691392"/>
+        <c:axId val="126870272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12000"/>
@@ -1028,17 +1022,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125693312"/>
+        <c:crossAx val="126872192"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
         <c:minorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125693312"/>
+        <c:axId val="126872192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="600"/>
+          <c:max val="650"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1081,14 +1075,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125691392"/>
+        <c:crossAx val="126870272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
         <c:minorUnit val="25"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126293504"/>
+        <c:axId val="149753856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1107,7 +1101,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Ratio</a:t>
+                  <a:t>Log	</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1115,18 +1109,18 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126295424"/>
+        <c:crossAx val="149549440"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
-        <c:minorUnit val="0.1"/>
+        <c:minorUnit val="0.25"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126295424"/>
+        <c:axId val="149549440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1136,8 +1130,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126293504"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="149753856"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -1206,7 +1199,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L2Rx10</c:v>
+                  <c:v> L2R10x</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1263,40 +1256,40 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>287.8</c:v>
+                  <c:v>358.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>710.1</c:v>
+                  <c:v>795.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1114</c:v>
+                  <c:v>1305.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1562.4</c:v>
+                  <c:v>1766.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1875.5</c:v>
+                  <c:v>2202.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2271.1999999999998</c:v>
+                  <c:v>2702.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2718.2</c:v>
+                  <c:v>3223.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3137.1</c:v>
+                  <c:v>3722.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3743.4</c:v>
+                  <c:v>4424.8999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4294.8</c:v>
+                  <c:v>5030.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4896.2</c:v>
+                  <c:v>5678.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5535.4</c:v>
+                  <c:v>6471</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1312,7 +1305,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> R2Lx10</c:v>
+                  <c:v> R2L10x</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1369,40 +1362,40 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>135.1</c:v>
+                  <c:v>164.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>162.30000000000001</c:v>
+                  <c:v>170.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>172</c:v>
+                  <c:v>187.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>172.8</c:v>
+                  <c:v>209.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>179.2</c:v>
+                  <c:v>212.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>182.9</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>187.5</c:v>
+                  <c:v>222.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>191.6</c:v>
+                  <c:v>227.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>193.8</c:v>
+                  <c:v>227.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>197.2</c:v>
+                  <c:v>233.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>199.6</c:v>
+                  <c:v>241.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>202.3</c:v>
+                  <c:v>242.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1417,8 +1410,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="37730176"/>
-        <c:axId val="128716800"/>
+        <c:axId val="127227776"/>
+        <c:axId val="127234048"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1428,7 +1421,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>test_10x_run!$H$1</c:f>
+              <c:f>test_10x_run!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1484,7 +1477,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>test_10x_run!$H$2:$H$13</c:f>
+              <c:f>test_10x_run!$G$2:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1537,11 +1530,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="128720896"/>
-        <c:axId val="128718720"/>
+        <c:axId val="127246336"/>
+        <c:axId val="127235968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37730176"/>
+        <c:axId val="127227776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120000"/>
@@ -1577,17 +1570,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128716800"/>
+        <c:crossAx val="127234048"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10000"/>
         <c:minorUnit val="5000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="128716800"/>
+        <c:axId val="127234048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6000"/>
+          <c:max val="6500"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1630,14 +1623,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37730176"/>
+        <c:crossAx val="127227776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1000"/>
         <c:minorUnit val="250"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="128718720"/>
+        <c:axId val="127235968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1656,7 +1649,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Ratio</a:t>
+                  <a:t>Log</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1666,16 +1659,16 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128720896"/>
+        <c:crossAx val="127246336"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
-        <c:minorUnit val="0.1"/>
+        <c:minorUnit val="0.25"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="128720896"/>
+        <c:axId val="127246336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,7 +1678,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128718720"/>
+        <c:crossAx val="127235968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1711,13 +1704,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>642939</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>14289</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>109538</xdr:rowOff>
@@ -1746,13 +1739,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>642939</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>14289</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>109538</xdr:rowOff>
@@ -2066,11 +2059,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -2080,37 +2071,33 @@
     <col min="4" max="4" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2118,27 +2105,23 @@
         <v>500</v>
       </c>
       <c r="C2">
-        <v>7500</v>
+        <v>10500</v>
       </c>
       <c r="D2">
-        <v>3330300</v>
-      </c>
-      <c r="E2" s="3">
-        <v>444</v>
+        <v>5481600</v>
+      </c>
+      <c r="E2" s="2">
+        <v>522.1</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4">
-        <f>ROUND(E2/E14, 3)</f>
-        <v>2.3260000000000001</v>
-      </c>
-      <c r="H2" s="5">
+      <c r="G2" s="3">
         <f>ROUND(B2*LOG(B2)/10000, 2)</f>
         <v>0.13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2146,27 +2129,23 @@
         <v>1500</v>
       </c>
       <c r="C3">
-        <v>22500</v>
+        <v>31500</v>
       </c>
       <c r="D3">
-        <v>10614000</v>
-      </c>
-      <c r="E3" s="3">
-        <v>471.7</v>
+        <v>13135100</v>
+      </c>
+      <c r="E3" s="2">
+        <v>417</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4">
-        <f t="shared" ref="G3:G13" si="0">ROUND(E3/E15, 3)</f>
-        <v>2.8130000000000002</v>
-      </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3:H13" si="1">ROUND(B3*LOG(B3)/10000, 2)</f>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G13" si="0">ROUND(B3*LOG(B3)/10000, 2)</f>
         <v>0.48</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2174,27 +2153,23 @@
         <v>2500</v>
       </c>
       <c r="C4">
-        <v>37500</v>
+        <v>52500</v>
       </c>
       <c r="D4">
-        <v>11075100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>295.3</v>
+        <v>25025000</v>
+      </c>
+      <c r="E4" s="2">
+        <v>476.7</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>1.9790000000000001</v>
-      </c>
-      <c r="H4" s="5">
-        <f t="shared" si="1"/>
         <v>0.85</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2202,27 +2177,23 @@
         <v>3500</v>
       </c>
       <c r="C5">
-        <v>52500</v>
+        <v>73500</v>
       </c>
       <c r="D5">
-        <v>17455400</v>
-      </c>
-      <c r="E5" s="3">
-        <v>332.5</v>
+        <v>21424200</v>
+      </c>
+      <c r="E5" s="2">
+        <v>291.5</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
-        <v>2.23</v>
-      </c>
-      <c r="H5" s="5">
-        <f t="shared" si="1"/>
         <v>1.24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2230,27 +2201,23 @@
         <v>4500</v>
       </c>
       <c r="C6">
-        <v>67500</v>
+        <v>94500</v>
       </c>
       <c r="D6">
-        <v>21494200</v>
-      </c>
-      <c r="E6" s="3">
-        <v>318.39999999999998</v>
+        <v>33542300</v>
+      </c>
+      <c r="E6" s="2">
+        <v>354.9</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
-        <v>2.11</v>
-      </c>
-      <c r="H6" s="5">
-        <f t="shared" si="1"/>
         <v>1.64</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2258,27 +2225,23 @@
         <v>5500</v>
       </c>
       <c r="C7">
-        <v>82500</v>
+        <v>115500</v>
       </c>
       <c r="D7">
-        <v>28505700</v>
-      </c>
-      <c r="E7" s="3">
-        <v>345.5</v>
+        <v>42812400</v>
+      </c>
+      <c r="E7" s="2">
+        <v>370.7</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>2.2989999999999999</v>
-      </c>
-      <c r="H7" s="5">
-        <f t="shared" si="1"/>
         <v>2.06</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2286,27 +2249,23 @@
         <v>6500</v>
       </c>
       <c r="C8">
-        <v>97500</v>
+        <v>136500</v>
       </c>
       <c r="D8">
-        <v>36823400</v>
-      </c>
-      <c r="E8" s="3">
-        <v>377.7</v>
+        <v>57053500</v>
+      </c>
+      <c r="E8" s="2">
+        <v>418</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>2.5049999999999999</v>
-      </c>
-      <c r="H8" s="5">
-        <f t="shared" si="1"/>
         <v>2.48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2314,27 +2273,23 @@
         <v>7500</v>
       </c>
       <c r="C9">
-        <v>112500</v>
+        <v>157500</v>
       </c>
       <c r="D9">
-        <v>45751300</v>
-      </c>
-      <c r="E9" s="3">
-        <v>406.7</v>
+        <v>75162800</v>
+      </c>
+      <c r="E9" s="2">
+        <v>477.2</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>2.6120000000000001</v>
-      </c>
-      <c r="H9" s="5">
-        <f t="shared" si="1"/>
         <v>2.91</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2342,27 +2297,23 @@
         <v>8500</v>
       </c>
       <c r="C10">
-        <v>127500</v>
+        <v>178500</v>
       </c>
       <c r="D10">
-        <v>59938700</v>
-      </c>
-      <c r="E10" s="3">
-        <v>470.1</v>
+        <v>87994600</v>
+      </c>
+      <c r="E10" s="2">
+        <v>493</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>3.0649999999999999</v>
-      </c>
-      <c r="H10" s="5">
-        <f t="shared" si="1"/>
         <v>3.34</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2370,27 +2321,23 @@
         <v>9500</v>
       </c>
       <c r="C11">
-        <v>142500</v>
+        <v>199500</v>
       </c>
       <c r="D11">
-        <v>69711800</v>
-      </c>
-      <c r="E11" s="3">
-        <v>489.2</v>
+        <v>102026400</v>
+      </c>
+      <c r="E11" s="2">
+        <v>511.4</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>3.2250000000000001</v>
-      </c>
-      <c r="H11" s="5">
-        <f t="shared" si="1"/>
         <v>3.78</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2398,27 +2345,23 @@
         <v>10500</v>
       </c>
       <c r="C12">
-        <v>157500</v>
+        <v>220500</v>
       </c>
       <c r="D12">
-        <v>85262000</v>
-      </c>
-      <c r="E12" s="3">
-        <v>541.29999999999995</v>
+        <v>124758300</v>
+      </c>
+      <c r="E12" s="2">
+        <v>565.79999999999995</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>3.52</v>
-      </c>
-      <c r="H12" s="5">
-        <f t="shared" si="1"/>
         <v>4.22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2426,27 +2369,23 @@
         <v>11500</v>
       </c>
       <c r="C13">
-        <v>172500</v>
-      </c>
-      <c r="D13" s="1">
-        <v>102873300</v>
-      </c>
-      <c r="E13" s="3">
-        <v>596.4</v>
+        <v>241500</v>
+      </c>
+      <c r="D13">
+        <v>150307200</v>
+      </c>
+      <c r="E13" s="2">
+        <v>622.4</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>3.657</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="1"/>
         <v>4.67</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2454,19 +2393,19 @@
         <v>500</v>
       </c>
       <c r="C14">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="D14">
-        <v>1718000</v>
-      </c>
-      <c r="E14" s="3">
-        <v>190.9</v>
+        <v>2072300</v>
+      </c>
+      <c r="E14" s="2">
+        <v>197.4</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2474,19 +2413,19 @@
         <v>1500</v>
       </c>
       <c r="C15">
-        <v>27000</v>
+        <v>31500</v>
       </c>
       <c r="D15">
-        <v>4529000</v>
-      </c>
-      <c r="E15" s="3">
-        <v>167.7</v>
+        <v>7076000</v>
+      </c>
+      <c r="E15" s="2">
+        <v>224.6</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2494,13 +2433,13 @@
         <v>2500</v>
       </c>
       <c r="C16">
-        <v>45000</v>
+        <v>52500</v>
       </c>
       <c r="D16">
-        <v>6714100</v>
-      </c>
-      <c r="E16" s="3">
-        <v>149.19999999999999</v>
+        <v>7970200</v>
+      </c>
+      <c r="E16" s="2">
+        <v>151.80000000000001</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -2514,13 +2453,13 @@
         <v>3500</v>
       </c>
       <c r="C17">
-        <v>63000</v>
+        <v>73500</v>
       </c>
       <c r="D17">
-        <v>9392600</v>
-      </c>
-      <c r="E17" s="3">
-        <v>149.1</v>
+        <v>11658000</v>
+      </c>
+      <c r="E17" s="2">
+        <v>158.6</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -2534,13 +2473,13 @@
         <v>4500</v>
       </c>
       <c r="C18">
-        <v>81000</v>
+        <v>94500</v>
       </c>
       <c r="D18">
-        <v>12224300</v>
-      </c>
-      <c r="E18" s="3">
-        <v>150.9</v>
+        <v>15380900</v>
+      </c>
+      <c r="E18" s="2">
+        <v>162.80000000000001</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -2554,13 +2493,13 @@
         <v>5500</v>
       </c>
       <c r="C19">
-        <v>99000</v>
+        <v>115500</v>
       </c>
       <c r="D19">
-        <v>14876000</v>
-      </c>
-      <c r="E19" s="3">
-        <v>150.30000000000001</v>
+        <v>17948900</v>
+      </c>
+      <c r="E19" s="2">
+        <v>155.4</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -2574,13 +2513,13 @@
         <v>6500</v>
       </c>
       <c r="C20">
-        <v>117000</v>
+        <v>136500</v>
       </c>
       <c r="D20">
-        <v>17644100</v>
-      </c>
-      <c r="E20" s="3">
-        <v>150.80000000000001</v>
+        <v>21269900</v>
+      </c>
+      <c r="E20" s="2">
+        <v>155.80000000000001</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -2594,13 +2533,13 @@
         <v>7500</v>
       </c>
       <c r="C21">
-        <v>135000</v>
+        <v>157500</v>
       </c>
       <c r="D21">
-        <v>21020500</v>
-      </c>
-      <c r="E21" s="3">
-        <v>155.69999999999999</v>
+        <v>27477200</v>
+      </c>
+      <c r="E21" s="2">
+        <v>174.5</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -2614,13 +2553,13 @@
         <v>8500</v>
       </c>
       <c r="C22">
-        <v>153000</v>
+        <v>178500</v>
       </c>
       <c r="D22">
-        <v>23471500</v>
-      </c>
-      <c r="E22" s="3">
-        <v>153.4</v>
+        <v>28441700</v>
+      </c>
+      <c r="E22" s="2">
+        <v>159.30000000000001</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -2634,13 +2573,13 @@
         <v>9500</v>
       </c>
       <c r="C23">
-        <v>171000</v>
+        <v>199500</v>
       </c>
       <c r="D23">
-        <v>25938600</v>
-      </c>
-      <c r="E23" s="3">
-        <v>151.69999999999999</v>
+        <v>33290500</v>
+      </c>
+      <c r="E23" s="2">
+        <v>166.9</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -2654,13 +2593,13 @@
         <v>10500</v>
       </c>
       <c r="C24">
-        <v>189000</v>
+        <v>220500</v>
       </c>
       <c r="D24">
-        <v>29077000</v>
-      </c>
-      <c r="E24" s="3">
-        <v>153.80000000000001</v>
+        <v>36990700</v>
+      </c>
+      <c r="E24" s="2">
+        <v>167.8</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -2674,13 +2613,13 @@
         <v>11500</v>
       </c>
       <c r="C25">
-        <v>207000</v>
+        <v>241500</v>
       </c>
       <c r="D25">
-        <v>33755200</v>
-      </c>
-      <c r="E25" s="3">
-        <v>163.1</v>
+        <v>40174700</v>
+      </c>
+      <c r="E25" s="2">
+        <v>166.4</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -2700,7 +2639,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2712,37 +2651,33 @@
     <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2750,27 +2685,23 @@
         <v>5000</v>
       </c>
       <c r="C2">
-        <v>75000</v>
+        <v>130000</v>
       </c>
       <c r="D2">
-        <v>21586600</v>
-      </c>
-      <c r="E2" s="3">
-        <v>287.8</v>
+        <v>46615700</v>
+      </c>
+      <c r="E2" s="2">
+        <v>358.6</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4">
-        <f>ROUND(E2/E14, 3)</f>
-        <v>2.13</v>
-      </c>
-      <c r="H2" s="5">
+      <c r="G2" s="3">
         <f>ROUND(B2*LOG(B2)/100000, 2)</f>
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2778,27 +2709,23 @@
         <v>15000</v>
       </c>
       <c r="C3">
-        <v>225000</v>
+        <v>390000</v>
       </c>
       <c r="D3">
-        <v>159778700</v>
-      </c>
-      <c r="E3" s="3">
-        <v>710.1</v>
+        <v>310267800</v>
+      </c>
+      <c r="E3" s="2">
+        <v>795.6</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4">
-        <f t="shared" ref="G3:G13" si="0">ROUND(E3/E15, 3)</f>
-        <v>4.375</v>
-      </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3:H13" si="1">ROUND(B3*LOG(B3)/100000, 2)</f>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G13" si="0">ROUND(B3*LOG(B3)/100000, 2)</f>
         <v>0.63</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2806,27 +2733,23 @@
         <v>25000</v>
       </c>
       <c r="C4">
-        <v>375000</v>
+        <v>650000</v>
       </c>
       <c r="D4">
-        <v>417757100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1114</v>
+        <v>848557500</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1305.5</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>6.4770000000000003</v>
-      </c>
-      <c r="H4" s="5">
-        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2834,27 +2757,23 @@
         <v>35000</v>
       </c>
       <c r="C5">
-        <v>525000</v>
+        <v>910000</v>
       </c>
       <c r="D5">
-        <v>820235400</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1562.4</v>
+        <v>1607214200</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1766.2</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
-        <v>9.0419999999999998</v>
-      </c>
-      <c r="H5" s="5">
-        <f t="shared" si="1"/>
         <v>1.59</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2862,27 +2781,23 @@
         <v>45000</v>
       </c>
       <c r="C6">
-        <v>675000</v>
+        <v>1170000</v>
       </c>
       <c r="D6">
-        <v>1265933700</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1875.5</v>
+        <v>2576676200</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2202.3000000000002</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
-        <v>10.465999999999999</v>
-      </c>
-      <c r="H6" s="5">
-        <f t="shared" si="1"/>
         <v>2.09</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2890,27 +2805,23 @@
         <v>55000</v>
       </c>
       <c r="C7">
-        <v>825000</v>
+        <v>1430000</v>
       </c>
       <c r="D7">
-        <v>1873753100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2271.1999999999998</v>
+        <v>3864193900</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2702.2</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>12.417999999999999</v>
-      </c>
-      <c r="H7" s="5">
-        <f t="shared" si="1"/>
         <v>2.61</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2918,27 +2829,23 @@
         <v>65000</v>
       </c>
       <c r="C8">
-        <v>975000</v>
+        <v>1690000</v>
       </c>
       <c r="D8">
-        <v>2650288900</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2718.2</v>
+        <v>5447447900</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3223.3</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>14.497</v>
-      </c>
-      <c r="H8" s="5">
-        <f t="shared" si="1"/>
         <v>3.13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2946,27 +2853,23 @@
         <v>75000</v>
       </c>
       <c r="C9">
-        <v>1125000</v>
+        <v>1950000</v>
       </c>
       <c r="D9">
-        <v>3529236000</v>
-      </c>
-      <c r="E9" s="3">
-        <v>3137.1</v>
+        <v>7258316300</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3722.2</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>16.373000000000001</v>
-      </c>
-      <c r="H9" s="5">
-        <f t="shared" si="1"/>
         <v>3.66</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2974,27 +2877,23 @@
         <v>85000</v>
       </c>
       <c r="C10">
-        <v>1275000</v>
+        <v>2210000</v>
       </c>
       <c r="D10">
-        <v>4772866200</v>
-      </c>
-      <c r="E10" s="3">
-        <v>3743.4</v>
+        <v>9779023300</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4424.8999999999996</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>19.315999999999999</v>
-      </c>
-      <c r="H10" s="5">
-        <f t="shared" si="1"/>
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3002,27 +2901,23 @@
         <v>95000</v>
       </c>
       <c r="C11">
-        <v>1425000</v>
+        <v>2470000</v>
       </c>
       <c r="D11">
-        <v>6120142300</v>
-      </c>
-      <c r="E11" s="3">
-        <v>4294.8</v>
+        <v>12424628200</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5030.2</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>21.779</v>
-      </c>
-      <c r="H11" s="5">
-        <f t="shared" si="1"/>
         <v>4.7300000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3030,27 +2925,23 @@
         <v>105000</v>
       </c>
       <c r="C12">
-        <v>1575000</v>
+        <v>2730000</v>
       </c>
       <c r="D12">
-        <v>7711560800</v>
-      </c>
-      <c r="E12" s="3">
-        <v>4896.2</v>
+        <v>15502345300</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5678.5</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>24.53</v>
-      </c>
-      <c r="H12" s="5">
-        <f t="shared" si="1"/>
         <v>5.27</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3058,27 +2949,23 @@
         <v>115000</v>
       </c>
       <c r="C13">
-        <v>1725000</v>
+        <v>2990000</v>
       </c>
       <c r="D13">
-        <v>9548554000</v>
-      </c>
-      <c r="E13" s="3">
-        <v>5535.4</v>
+        <v>19348309600</v>
+      </c>
+      <c r="E13" s="2">
+        <v>6471</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>27.361999999999998</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="1"/>
         <v>5.82</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3086,19 +2973,19 @@
         <v>5000</v>
       </c>
       <c r="C14">
-        <v>90000</v>
+        <v>155000</v>
       </c>
       <c r="D14">
-        <v>12159900</v>
-      </c>
-      <c r="E14" s="3">
-        <v>135.1</v>
+        <v>25500600</v>
+      </c>
+      <c r="E14" s="2">
+        <v>164.5</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3106,19 +2993,19 @@
         <v>15000</v>
       </c>
       <c r="C15">
-        <v>270000</v>
+        <v>465000</v>
       </c>
       <c r="D15">
-        <v>43818400</v>
-      </c>
-      <c r="E15" s="3">
-        <v>162.30000000000001</v>
+        <v>79197500</v>
+      </c>
+      <c r="E15" s="2">
+        <v>170.3</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3126,13 +3013,13 @@
         <v>25000</v>
       </c>
       <c r="C16">
-        <v>450000</v>
+        <v>775000</v>
       </c>
       <c r="D16">
-        <v>77415700</v>
-      </c>
-      <c r="E16" s="3">
-        <v>172</v>
+        <v>145400200</v>
+      </c>
+      <c r="E16" s="2">
+        <v>187.6</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -3146,13 +3033,13 @@
         <v>35000</v>
       </c>
       <c r="C17">
-        <v>630000</v>
+        <v>1085000</v>
       </c>
       <c r="D17">
-        <v>108845800</v>
-      </c>
-      <c r="E17" s="3">
-        <v>172.8</v>
+        <v>226951000</v>
+      </c>
+      <c r="E17" s="2">
+        <v>209.2</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -3166,13 +3053,13 @@
         <v>45000</v>
       </c>
       <c r="C18">
-        <v>810000</v>
+        <v>1395000</v>
       </c>
       <c r="D18">
-        <v>145117000</v>
-      </c>
-      <c r="E18" s="3">
-        <v>179.2</v>
+        <v>295969800</v>
+      </c>
+      <c r="E18" s="2">
+        <v>212.2</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -3186,13 +3073,13 @@
         <v>55000</v>
       </c>
       <c r="C19">
-        <v>990000</v>
+        <v>1705000</v>
       </c>
       <c r="D19">
-        <v>181065300</v>
-      </c>
-      <c r="E19" s="3">
-        <v>182.9</v>
+        <v>369983200</v>
+      </c>
+      <c r="E19" s="2">
+        <v>217</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -3206,13 +3093,13 @@
         <v>65000</v>
       </c>
       <c r="C20">
-        <v>1170000</v>
+        <v>2015000</v>
       </c>
       <c r="D20">
-        <v>219394800</v>
-      </c>
-      <c r="E20" s="3">
-        <v>187.5</v>
+        <v>448251200</v>
+      </c>
+      <c r="E20" s="2">
+        <v>222.5</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -3226,13 +3113,13 @@
         <v>75000</v>
       </c>
       <c r="C21">
-        <v>1350000</v>
+        <v>2325000</v>
       </c>
       <c r="D21">
-        <v>258666500</v>
-      </c>
-      <c r="E21" s="3">
-        <v>191.6</v>
+        <v>528304300</v>
+      </c>
+      <c r="E21" s="2">
+        <v>227.2</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -3246,13 +3133,13 @@
         <v>85000</v>
       </c>
       <c r="C22">
-        <v>1530000</v>
+        <v>2635000</v>
       </c>
       <c r="D22">
-        <v>296551900</v>
-      </c>
-      <c r="E22" s="3">
-        <v>193.8</v>
+        <v>598749500</v>
+      </c>
+      <c r="E22" s="2">
+        <v>227.2</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
@@ -3266,13 +3153,13 @@
         <v>95000</v>
       </c>
       <c r="C23">
-        <v>1710000</v>
+        <v>2945000</v>
       </c>
       <c r="D23">
-        <v>337168300</v>
-      </c>
-      <c r="E23" s="3">
-        <v>197.2</v>
+        <v>687876900</v>
+      </c>
+      <c r="E23" s="2">
+        <v>233.6</v>
       </c>
       <c r="F23" t="s">
         <v>12</v>
@@ -3286,13 +3173,13 @@
         <v>105000</v>
       </c>
       <c r="C24">
-        <v>1890000</v>
+        <v>3255000</v>
       </c>
       <c r="D24">
-        <v>377279800</v>
-      </c>
-      <c r="E24" s="3">
-        <v>199.6</v>
+        <v>786351300</v>
+      </c>
+      <c r="E24" s="2">
+        <v>241.6</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -3306,13 +3193,13 @@
         <v>115000</v>
       </c>
       <c r="C25">
-        <v>2070000</v>
+        <v>3565000</v>
       </c>
       <c r="D25">
-        <v>418787000</v>
-      </c>
-      <c r="E25" s="3">
-        <v>202.3</v>
+        <v>864039100</v>
+      </c>
+      <c r="E25" s="2">
+        <v>242.4</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>

</xml_diff>